<commit_message>
added quest phase tree and created first quest line with succes/failure path time to add saves and progress tracking
</commit_message>
<xml_diff>
--- a/zzz_other/tables.xlsx
+++ b/zzz_other/tables.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Filip\škola\!!!_MATRIP\DnD\zzz_other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBC2755-8D2D-4B12-92FB-149522E5DB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A28803-577E-42EE-BAAF-AC1173B7E4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{75D15189-BFBB-4142-B930-759327EB73F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{75D15189-BFBB-4142-B930-759327EB73F3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Předměty" sheetId="6" r:id="rId1"/>
-    <sheet name="Mise - fáze" sheetId="3" r:id="rId2"/>
-    <sheet name="Frakce" sheetId="8" r:id="rId3"/>
-    <sheet name="Postavy" sheetId="2" r:id="rId4"/>
-    <sheet name="Ulice" sheetId="1" r:id="rId5"/>
+    <sheet name="Ulice" sheetId="1" r:id="rId1"/>
+    <sheet name="Předměty" sheetId="6" r:id="rId2"/>
+    <sheet name="Mise - fáze" sheetId="3" r:id="rId3"/>
+    <sheet name="Frakce" sheetId="8" r:id="rId4"/>
+    <sheet name="Postavy" sheetId="2" r:id="rId5"/>
     <sheet name="Hráč" sheetId="5" r:id="rId6"/>
     <sheet name="Mise - linie" sheetId="7" r:id="rId7"/>
   </sheets>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="152">
   <si>
     <t>ID</t>
   </si>
@@ -495,6 +495,9 @@
   </si>
   <si>
     <t>Mečoun</t>
+  </si>
+  <si>
+    <t>Krátký meč</t>
   </si>
 </sst>
 </file>
@@ -855,10 +858,683 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9C1193-21D4-4077-9037-2F33601C62B1}">
+  <dimension ref="A1:I41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="1">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="1">
+        <v>29</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="1">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C38">
+    <sortCondition ref="A2:A38"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78C4A7C-2711-4806-8FFC-B45798D03982}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
@@ -1072,17 +1748,37 @@
         <v>15</v>
       </c>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11">
+        <v>-1</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1829089-82F1-4862-B7CA-2F568AF82BCB}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,7 +1903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56C8B259-0A78-4238-8F81-4979E459B12F}">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -1339,7 +2035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE42307A-777D-49E3-9DBB-1C926DF7AB9F}">
   <dimension ref="A1:H28"/>
   <sheetViews>
@@ -1409,7 +2105,7 @@
       </c>
       <c r="H2">
         <f ca="1">RANDBETWEEN(1,5-G2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1461,11 +2157,11 @@
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1489,11 +2185,11 @@
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1517,11 +2213,11 @@
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1545,7 +2241,7 @@
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
@@ -1573,11 +2269,11 @@
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1601,11 +2297,11 @@
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1629,7 +2325,7 @@
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
@@ -1657,11 +2353,11 @@
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1685,11 +2381,11 @@
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1717,7 +2413,7 @@
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1741,11 +2437,11 @@
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1769,11 +2465,11 @@
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1797,11 +2493,11 @@
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1829,7 +2525,7 @@
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1881,11 +2577,11 @@
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1937,7 +2633,7 @@
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
@@ -1965,11 +2661,11 @@
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2049,11 +2745,11 @@
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2077,7 +2773,7 @@
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
@@ -2109,7 +2805,7 @@
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2133,7 +2829,7 @@
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
@@ -2142,677 +2838,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9C1193-21D4-4077-9037-2F33601C62B1}">
-  <dimension ref="A1:I41"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="1">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>27</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>28</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>29</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>30</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>31</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="1">
-        <v>29</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>32</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>33</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>34</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>35</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>36</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>37</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>38</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40" s="1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>39</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C41" s="1">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C38">
-    <sortCondition ref="A2:A38"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added first characters and player saves
</commit_message>
<xml_diff>
--- a/zzz_other/tables.xlsx
+++ b/zzz_other/tables.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Filip\škola\!!!_MATRIP\DnD\zzz_other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A28803-577E-42EE-BAAF-AC1173B7E4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B070DBB-6954-4CFB-A209-B26030CD0DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{75D15189-BFBB-4142-B930-759327EB73F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{75D15189-BFBB-4142-B930-759327EB73F3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ulice" sheetId="1" r:id="rId1"/>
-    <sheet name="Předměty" sheetId="6" r:id="rId2"/>
-    <sheet name="Mise - fáze" sheetId="3" r:id="rId3"/>
-    <sheet name="Frakce" sheetId="8" r:id="rId4"/>
-    <sheet name="Postavy" sheetId="2" r:id="rId5"/>
+    <sheet name="Postavy" sheetId="2" r:id="rId1"/>
+    <sheet name="Ulice" sheetId="1" r:id="rId2"/>
+    <sheet name="Předměty" sheetId="6" r:id="rId3"/>
+    <sheet name="Mise - fáze" sheetId="3" r:id="rId4"/>
+    <sheet name="Frakce" sheetId="8" r:id="rId5"/>
     <sheet name="Hráč" sheetId="5" r:id="rId6"/>
     <sheet name="Mise - linie" sheetId="7" r:id="rId7"/>
   </sheets>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="153">
   <si>
     <t>ID</t>
   </si>
@@ -419,9 +419,6 @@
     <t>Nejvýše hledící</t>
   </si>
   <si>
-    <t>Biskup Svítání</t>
-  </si>
-  <si>
     <t>Nevnímající</t>
   </si>
   <si>
@@ -498,6 +495,12 @@
   </si>
   <si>
     <t>Krátký meč</t>
+  </si>
+  <si>
+    <t>coins</t>
+  </si>
+  <si>
+    <t>Biskup Třetího Úsvitu</t>
   </si>
 </sst>
 </file>
@@ -851,13 +854,931 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE42307A-777D-49E3-9DBB-1C926DF7AB9F}">
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>-1</v>
+      </c>
+      <c r="E2">
+        <v>32</v>
+      </c>
+      <c r="F2">
+        <v>-1</v>
+      </c>
+      <c r="G2">
+        <f ca="1">RANDBETWEEN(1,4)</f>
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <f ca="1">RANDBETWEEN(1,5-G2)</f>
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <f ca="1">RANDBETWEEN(0,20)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>-1</v>
+      </c>
+      <c r="E3">
+        <v>35</v>
+      </c>
+      <c r="F3">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G28" ca="1" si="0">RANDBETWEEN(1,4)</f>
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H28" ca="1" si="1">RANDBETWEEN(1,5-G3)</f>
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I28" ca="1" si="2">RANDBETWEEN(0,20)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>-1</v>
+      </c>
+      <c r="E4">
+        <v>35</v>
+      </c>
+      <c r="F4">
+        <v>35</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+      <c r="E5">
+        <v>35</v>
+      </c>
+      <c r="F5">
+        <v>35</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ca="1" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>-1</v>
+      </c>
+      <c r="E6">
+        <v>33</v>
+      </c>
+      <c r="F6">
+        <v>33</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>-1</v>
+      </c>
+      <c r="E7">
+        <v>34</v>
+      </c>
+      <c r="F7">
+        <v>34</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>-1</v>
+      </c>
+      <c r="E8">
+        <v>17</v>
+      </c>
+      <c r="F8">
+        <v>-1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ca="1" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>-1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>-1</v>
+      </c>
+      <c r="E10">
+        <v>13</v>
+      </c>
+      <c r="F10">
+        <v>-1</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>-1</v>
+      </c>
+      <c r="E11">
+        <v>23</v>
+      </c>
+      <c r="F11">
+        <v>23</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ca="1" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>-1</v>
+      </c>
+      <c r="E12">
+        <v>23</v>
+      </c>
+      <c r="F12">
+        <v>23</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>-1</v>
+      </c>
+      <c r="E13">
+        <v>37</v>
+      </c>
+      <c r="F13">
+        <v>37</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>-1</v>
+      </c>
+      <c r="E14">
+        <v>37</v>
+      </c>
+      <c r="F14">
+        <v>37</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>-1</v>
+      </c>
+      <c r="E15">
+        <v>37</v>
+      </c>
+      <c r="F15">
+        <v>37</v>
+      </c>
+      <c r="G15">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>-1</v>
+      </c>
+      <c r="E16">
+        <v>37</v>
+      </c>
+      <c r="F16">
+        <v>37</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>-1</v>
+      </c>
+      <c r="E17">
+        <v>37</v>
+      </c>
+      <c r="F17">
+        <v>37</v>
+      </c>
+      <c r="G17">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ca="1" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>-1</v>
+      </c>
+      <c r="E18">
+        <v>38</v>
+      </c>
+      <c r="F18">
+        <v>38</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>-1</v>
+      </c>
+      <c r="E19">
+        <v>38</v>
+      </c>
+      <c r="F19">
+        <v>38</v>
+      </c>
+      <c r="G19">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H19">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <f t="shared" ca="1" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>-1</v>
+      </c>
+      <c r="E20">
+        <v>38</v>
+      </c>
+      <c r="F20">
+        <v>38</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <f t="shared" ca="1" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>-1</v>
+      </c>
+      <c r="E21">
+        <v>38</v>
+      </c>
+      <c r="F21">
+        <v>38</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <f t="shared" ca="1" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>-1</v>
+      </c>
+      <c r="E22">
+        <v>38</v>
+      </c>
+      <c r="F22">
+        <v>38</v>
+      </c>
+      <c r="G22">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>-1</v>
+      </c>
+      <c r="E23">
+        <v>39</v>
+      </c>
+      <c r="F23">
+        <v>39</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <f t="shared" ca="1" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>-1</v>
+      </c>
+      <c r="E24">
+        <v>39</v>
+      </c>
+      <c r="F24">
+        <v>39</v>
+      </c>
+      <c r="G24">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>-1</v>
+      </c>
+      <c r="E25">
+        <v>39</v>
+      </c>
+      <c r="F25">
+        <v>39</v>
+      </c>
+      <c r="G25">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I25">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>-1</v>
+      </c>
+      <c r="E26">
+        <v>39</v>
+      </c>
+      <c r="F26">
+        <v>39</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>124</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>-1</v>
+      </c>
+      <c r="E27">
+        <v>39</v>
+      </c>
+      <c r="F27">
+        <v>39</v>
+      </c>
+      <c r="G27">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>-1</v>
+      </c>
+      <c r="E28">
+        <v>39</v>
+      </c>
+      <c r="F28">
+        <v>39</v>
+      </c>
+      <c r="G28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9C1193-21D4-4077-9037-2F33601C62B1}">
   <dimension ref="A1:I41"/>
   <sheetViews>
@@ -1530,7 +2451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78C4A7C-2711-4806-8FFC-B45798D03982}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -1559,13 +2480,13 @@
         <v>73</v>
       </c>
       <c r="D1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" t="s">
         <v>143</v>
       </c>
-      <c r="E1" t="s">
-        <v>144</v>
-      </c>
       <c r="F1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1633,10 +2554,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1653,10 +2574,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1673,10 +2594,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D7">
         <v>-1</v>
@@ -1693,10 +2614,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D8">
         <v>-1</v>
@@ -1713,7 +2634,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C9" t="s">
         <v>74</v>
@@ -1733,10 +2654,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D10">
         <v>-1</v>
@@ -1753,10 +2674,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D11">
         <v>-1</v>
@@ -1773,11 +2694,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1829089-82F1-4862-B7CA-2F568AF82BCB}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
@@ -1807,7 +2728,7 @@
         <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1829,7 +2750,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1840,7 +2761,7 @@
         <v>67</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1848,10 +2769,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1859,10 +2780,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1870,7 +2791,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>74</v>
@@ -1881,7 +2802,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>74</v>
@@ -1892,10 +2813,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1903,7 +2824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56C8B259-0A78-4238-8F81-4979E459B12F}">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -1942,7 +2863,7 @@
         <v>35</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1956,7 +2877,7 @@
         <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1970,7 +2891,7 @@
         <v>38</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1984,7 +2905,7 @@
         <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1998,7 +2919,7 @@
         <v>-1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2012,7 +2933,7 @@
         <v>-1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2020,824 +2941,18 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C8" s="1">
         <v>-1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE42307A-777D-49E3-9DBB-1C926DF7AB9F}">
-  <dimension ref="A1:H28"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" t="s">
-        <v>148</v>
-      </c>
-      <c r="H1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>-1</v>
-      </c>
-      <c r="E2">
-        <v>32</v>
-      </c>
-      <c r="F2">
-        <v>-1</v>
-      </c>
-      <c r="G2">
-        <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <f ca="1">RANDBETWEEN(1,5-G2)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>-1</v>
-      </c>
-      <c r="E3">
-        <v>35</v>
-      </c>
-      <c r="F3">
-        <v>14</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G28" ca="1" si="0">RANDBETWEEN(1,4)</f>
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H28" ca="1" si="1">RANDBETWEEN(1,5-G3)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>-1</v>
-      </c>
-      <c r="E4">
-        <v>35</v>
-      </c>
-      <c r="F4">
-        <v>35</v>
-      </c>
-      <c r="G4">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>-1</v>
-      </c>
-      <c r="E5">
-        <v>35</v>
-      </c>
-      <c r="F5">
-        <v>35</v>
-      </c>
-      <c r="G5">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>-1</v>
-      </c>
-      <c r="E6">
-        <v>33</v>
-      </c>
-      <c r="F6">
-        <v>33</v>
-      </c>
-      <c r="G6">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H6">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>-1</v>
-      </c>
-      <c r="E7">
-        <v>34</v>
-      </c>
-      <c r="F7">
-        <v>34</v>
-      </c>
-      <c r="G7">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H7">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>-1</v>
-      </c>
-      <c r="E8">
-        <v>17</v>
-      </c>
-      <c r="F8">
-        <v>-1</v>
-      </c>
-      <c r="G8">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H8">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>-1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>107</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>-1</v>
-      </c>
-      <c r="E10">
-        <v>13</v>
-      </c>
-      <c r="F10">
-        <v>-1</v>
-      </c>
-      <c r="G10">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>108</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11">
-        <v>-1</v>
-      </c>
-      <c r="E11">
-        <v>23</v>
-      </c>
-      <c r="F11">
-        <v>23</v>
-      </c>
-      <c r="G11">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H11">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>109</v>
-      </c>
-      <c r="C12">
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <v>-1</v>
-      </c>
-      <c r="E12">
-        <v>23</v>
-      </c>
-      <c r="F12">
-        <v>23</v>
-      </c>
-      <c r="G12">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>-1</v>
-      </c>
-      <c r="E13">
-        <v>37</v>
-      </c>
-      <c r="F13">
-        <v>37</v>
-      </c>
-      <c r="G13">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>111</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>-1</v>
-      </c>
-      <c r="E14">
-        <v>37</v>
-      </c>
-      <c r="F14">
-        <v>37</v>
-      </c>
-      <c r="G14">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>112</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>-1</v>
-      </c>
-      <c r="E15">
-        <v>37</v>
-      </c>
-      <c r="F15">
-        <v>37</v>
-      </c>
-      <c r="G15">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H15">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>113</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>-1</v>
-      </c>
-      <c r="E16">
-        <v>37</v>
-      </c>
-      <c r="F16">
-        <v>37</v>
-      </c>
-      <c r="G16">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H16">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>114</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>-1</v>
-      </c>
-      <c r="E17">
-        <v>37</v>
-      </c>
-      <c r="F17">
-        <v>37</v>
-      </c>
-      <c r="G17">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H17">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>115</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18">
-        <v>-1</v>
-      </c>
-      <c r="E18">
-        <v>38</v>
-      </c>
-      <c r="F18">
-        <v>38</v>
-      </c>
-      <c r="G18">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H18">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>116</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19">
-        <v>-1</v>
-      </c>
-      <c r="E19">
-        <v>38</v>
-      </c>
-      <c r="F19">
-        <v>38</v>
-      </c>
-      <c r="G19">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H19">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20">
-        <v>-1</v>
-      </c>
-      <c r="E20">
-        <v>38</v>
-      </c>
-      <c r="F20">
-        <v>38</v>
-      </c>
-      <c r="G20">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H20">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>118</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21">
-        <v>-1</v>
-      </c>
-      <c r="E21">
-        <v>38</v>
-      </c>
-      <c r="F21">
-        <v>38</v>
-      </c>
-      <c r="G21">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H21">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>119</v>
-      </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22">
-        <v>-1</v>
-      </c>
-      <c r="E22">
-        <v>38</v>
-      </c>
-      <c r="F22">
-        <v>38</v>
-      </c>
-      <c r="G22">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H22">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>120</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="D23">
-        <v>-1</v>
-      </c>
-      <c r="E23">
-        <v>39</v>
-      </c>
-      <c r="F23">
-        <v>39</v>
-      </c>
-      <c r="G23">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H23">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>121</v>
-      </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
-      <c r="D24">
-        <v>-1</v>
-      </c>
-      <c r="E24">
-        <v>39</v>
-      </c>
-      <c r="F24">
-        <v>39</v>
-      </c>
-      <c r="G24">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H24">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>122</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-      <c r="D25">
-        <v>-1</v>
-      </c>
-      <c r="E25">
-        <v>39</v>
-      </c>
-      <c r="F25">
-        <v>39</v>
-      </c>
-      <c r="G25">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H25">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>123</v>
-      </c>
-      <c r="C26">
-        <v>3</v>
-      </c>
-      <c r="D26">
-        <v>-1</v>
-      </c>
-      <c r="E26">
-        <v>39</v>
-      </c>
-      <c r="F26">
-        <v>39</v>
-      </c>
-      <c r="G26">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H26">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>124</v>
-      </c>
-      <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="D27">
-        <v>-1</v>
-      </c>
-      <c r="E27">
-        <v>39</v>
-      </c>
-      <c r="F27">
-        <v>39</v>
-      </c>
-      <c r="G27">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H27">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>125</v>
-      </c>
-      <c r="C28">
-        <v>3</v>
-      </c>
-      <c r="D28">
-        <v>-1</v>
-      </c>
-      <c r="E28">
-        <v>39</v>
-      </c>
-      <c r="F28">
-        <v>39</v>
-      </c>
-      <c r="G28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H28">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
implemented fight for characters but you can kill dead characters
</commit_message>
<xml_diff>
--- a/zzz_other/tables.xlsx
+++ b/zzz_other/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Filip\škola\!!!_MATRIP\DnD\zzz_other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B070DBB-6954-4CFB-A209-B26030CD0DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFB72E7-F644-4E71-BF0A-E2D149EA342E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{75D15189-BFBB-4142-B930-759327EB73F3}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="158">
   <si>
     <t>ID</t>
   </si>
@@ -501,6 +501,21 @@
   </si>
   <si>
     <t>Biskup Třetího Úsvitu</t>
+  </si>
+  <si>
+    <t>Jimmy Děravý Koleno</t>
+  </si>
+  <si>
+    <t>Pedro Wellington</t>
+  </si>
+  <si>
+    <t>Zesty Bergamot</t>
+  </si>
+  <si>
+    <t>Tewkesbury</t>
+  </si>
+  <si>
+    <t>Malý Rhompson</t>
   </si>
 </sst>
 </file>
@@ -862,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE42307A-777D-49E3-9DBB-1C926DF7AB9F}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,11 +945,11 @@
       </c>
       <c r="G2">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <f ca="1">RANDBETWEEN(1,5-G2)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I2">
         <f ca="1">RANDBETWEEN(0,20)</f>
@@ -961,16 +976,16 @@
         <v>14</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G28" ca="1" si="0">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <f t="shared" ref="G3:G33" ca="1" si="0">RANDBETWEEN(1,4)</f>
+        <v>4</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H28" ca="1" si="1">RANDBETWEEN(1,5-G3)</f>
-        <v>2</v>
+        <f t="shared" ref="H3:H33" ca="1" si="1">RANDBETWEEN(1,5-G3)</f>
+        <v>1</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I28" ca="1" si="2">RANDBETWEEN(0,20)</f>
-        <v>15</v>
+        <f t="shared" ref="I3:I33" ca="1" si="2">RANDBETWEEN(0,20)</f>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -994,7 +1009,7 @@
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
@@ -1002,7 +1017,7 @@
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1034,7 +1049,7 @@
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1058,15 +1073,15 @@
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1090,7 +1105,7 @@
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
@@ -1098,7 +1113,7 @@
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1130,7 +1145,7 @@
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1154,7 +1169,7 @@
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
@@ -1162,7 +1177,7 @@
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1186,7 +1201,7 @@
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
@@ -1194,7 +1209,7 @@
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1218,15 +1233,15 @@
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1250,7 +1265,7 @@
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
@@ -1258,7 +1273,7 @@
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1282,15 +1297,15 @@
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1322,7 +1337,7 @@
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1346,15 +1361,15 @@
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1378,7 +1393,7 @@
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="1"/>
@@ -1386,7 +1401,7 @@
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1410,15 +1425,15 @@
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1442,15 +1457,15 @@
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1474,7 +1489,7 @@
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
@@ -1482,7 +1497,7 @@
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1506,15 +1521,15 @@
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1538,7 +1553,7 @@
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
@@ -1546,7 +1561,7 @@
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1570,7 +1585,7 @@
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
@@ -1578,7 +1593,7 @@
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1602,7 +1617,7 @@
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
@@ -1610,7 +1625,7 @@
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1634,15 +1649,15 @@
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1674,7 +1689,7 @@
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1698,15 +1713,15 @@
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1730,7 +1745,7 @@
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
@@ -1738,7 +1753,7 @@
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1762,15 +1777,175 @@
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>153</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>-1</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29">
+        <v>7</v>
+      </c>
+      <c r="G29">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I29">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>154</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>-1</v>
+      </c>
+      <c r="E30">
+        <v>7</v>
+      </c>
+      <c r="F30">
+        <v>7</v>
+      </c>
+      <c r="G30">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H30">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>155</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>-1</v>
+      </c>
+      <c r="E31">
+        <v>7</v>
+      </c>
+      <c r="F31">
+        <v>7</v>
+      </c>
+      <c r="G31">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H31">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <f t="shared" ca="1" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>-1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H32">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>157</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>-1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I33">
+        <f t="shared" ca="1" si="2"/>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1782,7 +1957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9C1193-21D4-4077-9037-2F33601C62B1}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
save before adding dynamic character search
</commit_message>
<xml_diff>
--- a/zzz_other/tables.xlsx
+++ b/zzz_other/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Filip\škola\!!!_MATRIP\DnD\zzz_other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFB72E7-F644-4E71-BF0A-E2D149EA342E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C54F673-7C88-4EAE-AD19-7550D959A3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{75D15189-BFBB-4142-B930-759327EB73F3}"/>
+    <workbookView xWindow="29325" yWindow="5220" windowWidth="15030" windowHeight="13290" activeTab="3" xr2:uid="{75D15189-BFBB-4142-B930-759327EB73F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Postavy" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="162">
   <si>
     <t>ID</t>
   </si>
@@ -516,6 +516,18 @@
   </si>
   <si>
     <t>Malý Rhompson</t>
+  </si>
+  <si>
+    <t>Kradmá Thalastra</t>
+  </si>
+  <si>
+    <t>Momo Lotter</t>
+  </si>
+  <si>
+    <t>Tomáš Víčko</t>
+  </si>
+  <si>
+    <t>Nastrč</t>
   </si>
 </sst>
 </file>
@@ -877,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE42307A-777D-49E3-9DBB-1C926DF7AB9F}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,11 +961,11 @@
       </c>
       <c r="H2">
         <f ca="1">RANDBETWEEN(1,5-G2)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I2">
         <f ca="1">RANDBETWEEN(0,20)</f>
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -976,16 +988,16 @@
         <v>14</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G33" ca="1" si="0">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <f t="shared" ref="G3:G36" ca="1" si="0">RANDBETWEEN(1,4)</f>
+        <v>3</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H33" ca="1" si="1">RANDBETWEEN(1,5-G3)</f>
-        <v>1</v>
+        <f t="shared" ref="H3:H36" ca="1" si="1">RANDBETWEEN(1,5-G3)</f>
+        <v>2</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I33" ca="1" si="2">RANDBETWEEN(0,20)</f>
-        <v>18</v>
+        <f t="shared" ref="I3:I36" ca="1" si="2">RANDBETWEEN(0,20)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1009,15 +1021,15 @@
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1049,7 +1061,7 @@
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1073,15 +1085,15 @@
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1109,11 +1121,11 @@
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1169,15 +1181,15 @@
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1205,11 +1217,11 @@
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1233,7 +1245,7 @@
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
@@ -1241,7 +1253,7 @@
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1265,15 +1277,15 @@
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1297,15 +1309,15 @@
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1329,15 +1341,15 @@
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1361,15 +1373,15 @@
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1393,7 +1405,7 @@
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="1"/>
@@ -1401,7 +1413,7 @@
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1425,15 +1437,15 @@
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1457,15 +1469,15 @@
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1489,7 +1501,7 @@
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
@@ -1497,7 +1509,7 @@
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1521,7 +1533,7 @@
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
@@ -1529,7 +1541,7 @@
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1553,15 +1565,15 @@
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1593,7 +1605,7 @@
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1617,15 +1629,15 @@
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1649,11 +1661,11 @@
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="2"/>
@@ -1681,7 +1693,7 @@
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
@@ -1689,7 +1701,7 @@
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1713,15 +1725,15 @@
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1753,7 +1765,7 @@
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1777,15 +1789,15 @@
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1809,15 +1821,15 @@
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1841,7 +1853,7 @@
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
@@ -1849,7 +1861,7 @@
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1873,7 +1885,7 @@
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="1"/>
@@ -1881,7 +1893,7 @@
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1905,7 +1917,7 @@
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="1"/>
@@ -1913,7 +1925,7 @@
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1937,15 +1949,111 @@
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>158</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>-1</v>
+      </c>
+      <c r="E34">
+        <v>19</v>
+      </c>
+      <c r="F34">
+        <v>3</v>
+      </c>
+      <c r="G34">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H34">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <f t="shared" ca="1" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>159</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>-1</v>
+      </c>
+      <c r="E35">
+        <v>20</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+      <c r="G35">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I35">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>160</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>-1</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H36">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I36">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2871,10 +2979,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1829089-82F1-4862-B7CA-2F568AF82BCB}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2992,6 +3100,17 @@
       </c>
       <c r="C10" s="2" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started handling character input
</commit_message>
<xml_diff>
--- a/zzz_other/tables.xlsx
+++ b/zzz_other/tables.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Filip\škola\!!!_MATRIP\DnD\zzz_other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C54F673-7C88-4EAE-AD19-7550D959A3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA30D4D-D4ED-4668-8917-0810B6318D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29325" yWindow="5220" windowWidth="15030" windowHeight="13290" activeTab="3" xr2:uid="{75D15189-BFBB-4142-B930-759327EB73F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{75D15189-BFBB-4142-B930-759327EB73F3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Postavy" sheetId="2" r:id="rId1"/>
-    <sheet name="Ulice" sheetId="1" r:id="rId2"/>
+    <sheet name="Ulice" sheetId="1" r:id="rId1"/>
+    <sheet name="Postavy" sheetId="2" r:id="rId2"/>
     <sheet name="Předměty" sheetId="6" r:id="rId3"/>
     <sheet name="Mise - fáze" sheetId="3" r:id="rId4"/>
     <sheet name="Frakce" sheetId="8" r:id="rId5"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="204">
   <si>
     <t>ID</t>
   </si>
@@ -528,6 +528,132 @@
   </si>
   <si>
     <t>Nastrč</t>
+  </si>
+  <si>
+    <t>Dlážděná ulice Svobodnické ulice se klikatí srdcem města, míjející vysoké kamenné budovy a třpytivé kouzelné lucerny.</t>
+  </si>
+  <si>
+    <t>description_cz</t>
+  </si>
+  <si>
+    <t>Ostrá ulice je temnou a úzkou pasáží, zarostlou liánami, jež lemují rozpadající se zdi.</t>
+  </si>
+  <si>
+    <t>Ve vzduchu visí tíživý pocit neklidu a nebezpečí.</t>
+  </si>
+  <si>
+    <t>Vznešená třída je krásná alej s křišťálově lesklou dlažbou, obklopená čistě bílými budovami.</t>
+  </si>
+  <si>
+    <t>Zakopaná ulice je ponurá a zamlžená ulice, zahalená tmou a plná nevyzpytatelného šepotu.</t>
+  </si>
+  <si>
+    <t>Ezoterická ulice je rozmarná ulice plná pestrobarevně malovaných fasád a s  podivným zápachem magie ve vzduchu.</t>
+  </si>
+  <si>
+    <t>Vyčichlá ulice je podivné místo, kde tančí podivné stíny a ozývá se strašidelný šepot.</t>
+  </si>
+  <si>
+    <t>Náměstí páně je velké otevřené náměstí obklopené prodejci nejrůznorodějších produktů, ručně vyráběného zboží a mnoha dalšího.</t>
+  </si>
+  <si>
+    <t>Třída vykoupení je ulice s velkolepou architekturou a širokými chodníky, lemovaná luxusními obchody.</t>
+  </si>
+  <si>
+    <t>Slaná je nejrušnější přístavní ulicí. Přes všechny handrkující se rybáře člověk skoro neslyší své vlastní myšlenky.</t>
+  </si>
+  <si>
+    <t>Perlová ulice je navzdory svému názvu známá pro hospody s velice levným alkoholem.</t>
+  </si>
+  <si>
+    <t>Bahno je úzká, nedlážděná ulice lemovaná chatrnými dřevěnými boudami a potulujícími se slepicemi.</t>
+  </si>
+  <si>
+    <t>Strmá ulice je lemovaná kovářskými dílnami, kde zvoní kladiva při výrobě zbraní a nástrojů.</t>
+  </si>
+  <si>
+    <t>Jílová ulice je plna štiplavého zápachu kůže a člověk si snadno domyslí, že se zde zpracovávají zvířecí kůže a vyrábí se z nich všemožné zboží.</t>
+  </si>
+  <si>
+    <t>Ulice U kotvy a ráhna se vine podél přístavu, plná úlovků, které jsou přiváženy z moře.</t>
+  </si>
+  <si>
+    <t>Rajská je ulice lemovaná cihlovými domy, z jejichž komínů se line vůně dřevěného kouře.</t>
+  </si>
+  <si>
+    <t>Hluchá je ulice plná dřevěných domů, jejichž zdi jsou zvětralé a šedivé.</t>
+  </si>
+  <si>
+    <t>Cedrová ulice je plná domů obložených cedrovým dřevem, jejichž verandy a balkony poskytují úkryt před zapadjícím sluncem.</t>
+  </si>
+  <si>
+    <t>Provaznická je ulice plná domů s doškovými střechami a dlážděnou silnicí.</t>
+  </si>
+  <si>
+    <t>Nasátá je ulice plná domů obklopených břečťanem, jejichž zdi pokrývají zelené liány.</t>
+  </si>
+  <si>
+    <t>Jízda je ulice lemovaná honosnými domy z mramoru, jejichž sloupy a oblouky dodávají ulici na eleganci.</t>
+  </si>
+  <si>
+    <t>Spojovací je ulice plná domů ze žuly, jejichž zdi jsou šedé a robustní.</t>
+  </si>
+  <si>
+    <t>Kořenová ulice je plná skromných domů s pevně zavřenými okny a dveřmi.</t>
+  </si>
+  <si>
+    <t>Bulvár spásy je ulice plná úhledných domů s čistě zametenými prahy a vyleštěnými okny.</t>
+  </si>
+  <si>
+    <t>Smečky jsou ulicí plnou domů, jejichž klid je ideálním místem k odpočinku a relaxaci.</t>
+  </si>
+  <si>
+    <t>Ulice Poslední naděje je lemovaná domy s malými dveřmi a okny, jejichž komíny sahají vysoko k nebi.</t>
+  </si>
+  <si>
+    <t>Nekonečná je ulice plná domů, jejichž dveře a okna pokrývá silná vrstva prachu z každodenního ruchu města.</t>
+  </si>
+  <si>
+    <t>Obludná ulice je lemovaná domy, jejichž zdi vykazují známky stárnutí a střechy se prohýbají.</t>
+  </si>
+  <si>
+    <t>Padlá ulice je plná domů s kamennými zdmi a doškovými střechami, jednoduchými, ale pevnými.</t>
+  </si>
+  <si>
+    <t>Bílý trh je rušná oblast plná prodejců nejrůznějšího zboží, od ovoce a zeleniny až po exotické koření a cetky. Skutečná tvář trhu se však skrývá v jeho špinavém podhoubí, kde prodejci obchodují s kradeným zbožím, nelegálním zbožím a dalším ne zrovna čestným zbožím.</t>
+  </si>
+  <si>
+    <t>Měsíční je ulice plná domů, jejichž zdi jsou zjizvené léty opotřebení.</t>
+  </si>
+  <si>
+    <t>Nad městem se tyčí hrad, jehož hradby a věže jsou ze zvětralého kamene. Hrad stojí již po staletí a jeho historie se vryla do jeho zdí a cimbuří. Čas se na hradu podepsal, jeho zdi a věže vykazují známky stáří a opotřebení, ale jeho pevná konstrukce ho udržela na nohou, což svědčí o síle a odhodlání těch, kteří ho postavili.</t>
+  </si>
+  <si>
+    <t>Poslední brána je hlavním vstupem do města a její masivní železné dveře se tyčí nad všemi, kdo jimi procházejí. Brána je střežena ve dne v noci a jeji železné mříže jsou symbolem síly a ochrany města.</t>
+  </si>
+  <si>
+    <t>Temná brána, ač názvem nevypovídající, je krásným vstupem do města, jehož kamenné zdi zdobí složité řezby a pozlacené akcenty. Oblouk je symbolem bohatství a prosperity města a jeho krása přitahuje návštěvníky z blízka i daleka.</t>
+  </si>
+  <si>
+    <t>Před stanicí stojí skupina strážců, kteří sledují město pod sebou a dávají pozor na jakékoli známky problémů. Stanice je vybavena zvonem, kterým lze v případě nouze vyhlásit poplach. Strážní stanice slouží jako první linie obrany města, její strážci jsou neustále ve střehu, chrání občany a udržují pořádek.</t>
+  </si>
+  <si>
+    <t>Výrobna šňupce je malá, nenápadná budova v tiché uličce. Okna jsou pokrytá špínou, dveře pevně zamčené, což vyvolává dojem, že je opuštěná. Uvnitř však probíhá rušný provoz, dělníci míchají a vaří různé drogy a lektvary. Navzdory nebezpečí fabrika dál vyrábí své zboží a zásobuje černý trh stálým přísunem nelegálních drog.</t>
+  </si>
+  <si>
+    <t>Doupě Smradlavých hlav se nachází v samém srdci přístavu a jeho vchod je skrytý za hromadou beden a sudů. Doupě je úlem plným aktivit, členové gangu přicházejí a odcházejí v každou denní i noční hodinu. Interiér je spoře osvětlený, s hrubými dřevěnými stěnami a špinavou podlahou. Členové gangu se shromažďují kolem velkého stolu uprostřed místnosti, kde probírají své nejnovější plány a plánují další operace.</t>
+  </si>
+  <si>
+    <t>Úkryt Rudého klanu se nachází v samém srdci města, ukrytý ve spleti temných uliček a stísněných ulic. Vchod hlídá skupina drsně vyhlížejících bouchačů, kteří očima zkoumají okolí a hledají jakýkoli náznak potíží. Uvnitř úkrytu panuje čilý ruch, členové gangu přicházejí a odcházejí, plánují další kroky a rozdělují si zisk z posledních zločinů. Stěny jsou pokryty graffiti, která označují území gangu a ukazují jeho nadvládu nad okolím. Úkryt je místem moci a strachu, centrem jednoho z nejnebezpečnějších gangů ve městě.</t>
+  </si>
+  <si>
+    <t>Kostel Prvního očištění stojí na Náměstí Páně a nelze jej přehlédnout. Jeho kdysi velkolepá fasáda je nyní zvětralá a zarostlá vinnou révou. Kostel je již mnoho let opuštěný, jeho dveře jsou zamčené a okna zabedněná. Nicméně za těmito dveřmi se usídlila temná a zlověstná síla. Náboženští fanatici si kostel přivlastnili a využívají jeho sály jako základnu, odkud uskutečňují své zvrácené plány. Stěny jsou vyzdobeny zlověstnými symboly a vzduch je prosycen vůní kadidla a zvukem zpěvu. Zapomenutý kostel se stal místem strachu, protože ho fanatici využívají k šíření svého poselství a získávání přívrženců.</t>
+  </si>
+  <si>
+    <t>possibilities</t>
+  </si>
+  <si>
+    <t>Opilý poník je hlučná hospoda v centru města. Její stěny jsou z hrubě opracovaného kamene a střecha je pokrytá slámou. Uvnitř je hospoda hlučná a bujará, podél jedné stěny se táhne velký bar a na druhé straně doutná krb. Barmani jsou nevrlí a rychle obsluhují, zatímco hosté jsou neurvalá parta, která křičí a směje se za zvuků řinčení sklenic a vrzání prken. Jídelní lístek v restauraci The Drunken Pony se skládá převážně z vydatných dušených jídel a masa, které se zapíjejí velkými hrnky pěnivého piva. Krčma je oblíbeným místem cestovatelů, obchodníků i místních obyvatel, kteří sem chodí popíjet, vyprávět si příběhy a sdílet kamarádství na cestách.</t>
   </si>
 </sst>
 </file>
@@ -564,7 +690,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -574,6 +700,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -888,6 +1020,773 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9C1193-21D4-4077-9037-2F33601C62B1}">
+  <dimension ref="A1:I41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="1">
+        <v>20</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="1">
+        <v>29</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="1">
+        <v>27</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="1">
+        <v>12</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="1">
+        <v>5</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="1">
+        <v>3</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="1">
+        <v>28</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="1">
+        <v>15</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C38">
+    <sortCondition ref="A2:A38"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE42307A-777D-49E3-9DBB-1C926DF7AB9F}">
   <dimension ref="A1:I36"/>
   <sheetViews>
@@ -957,7 +1856,7 @@
       </c>
       <c r="G2">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2">
         <f ca="1">RANDBETWEEN(1,5-G2)</f>
@@ -989,15 +1888,15 @@
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G36" ca="1" si="0">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H36" ca="1" si="1">RANDBETWEEN(1,5-G3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I36" ca="1" si="2">RANDBETWEEN(0,20)</f>
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1021,7 +1920,7 @@
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
@@ -1029,7 +1928,7 @@
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1053,7 +1952,7 @@
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
@@ -1061,7 +1960,7 @@
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1085,7 +1984,7 @@
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
@@ -1093,7 +1992,7 @@
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1117,15 +2016,15 @@
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1157,7 +2056,7 @@
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1185,11 +2084,11 @@
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1213,7 +2112,7 @@
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
@@ -1221,7 +2120,7 @@
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1249,11 +2148,11 @@
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1277,15 +2176,15 @@
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1309,15 +2208,15 @@
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1341,7 +2240,7 @@
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="1"/>
@@ -1349,7 +2248,7 @@
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1373,15 +2272,15 @@
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1405,7 +2304,7 @@
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="1"/>
@@ -1413,7 +2312,7 @@
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1437,7 +2336,7 @@
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
@@ -1445,7 +2344,7 @@
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1473,11 +2372,11 @@
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1501,15 +2400,15 @@
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1537,11 +2436,11 @@
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1569,11 +2468,11 @@
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1597,7 +2496,7 @@
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
@@ -1605,7 +2504,7 @@
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1629,15 +2528,15 @@
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1661,15 +2560,15 @@
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1693,11 +2592,11 @@
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="2"/>
@@ -1733,7 +2632,7 @@
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1757,15 +2656,15 @@
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1789,7 +2688,7 @@
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
@@ -1797,7 +2696,7 @@
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1821,15 +2720,15 @@
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1853,7 +2752,7 @@
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
@@ -1861,7 +2760,7 @@
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1885,15 +2784,15 @@
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1917,7 +2816,7 @@
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="1"/>
@@ -1925,7 +2824,7 @@
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1949,7 +2848,7 @@
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="1"/>
@@ -1957,7 +2856,7 @@
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1989,7 +2888,7 @@
       </c>
       <c r="I34">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2013,15 +2912,15 @@
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2045,692 +2944,19 @@
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I36">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9C1193-21D4-4077-9037-2F33601C62B1}">
-  <dimension ref="A1:I41"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="1">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>27</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>28</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>29</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>30</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>31</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="1">
-        <v>29</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>32</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>33</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>34</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>35</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>36</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>37</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>38</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40" s="1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>39</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C41" s="1">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C38">
-    <sortCondition ref="A2:A38"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2981,7 +3207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1829089-82F1-4862-B7CA-2F568AF82BCB}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
reworked items and streets csv files
</commit_message>
<xml_diff>
--- a/zzz_other/tables.xlsx
+++ b/zzz_other/tables.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Filip\škola\!!!_MATRIP\DnD\zzz_other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA30D4D-D4ED-4668-8917-0810B6318D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EE255F-AFF1-42F0-A9F4-47F29B5A1AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{75D15189-BFBB-4142-B930-759327EB73F3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ulice" sheetId="1" r:id="rId1"/>
-    <sheet name="Postavy" sheetId="2" r:id="rId2"/>
-    <sheet name="Předměty" sheetId="6" r:id="rId3"/>
+    <sheet name="Předměty" sheetId="6" r:id="rId1"/>
+    <sheet name="Ulice" sheetId="1" r:id="rId2"/>
+    <sheet name="Postavy" sheetId="2" r:id="rId3"/>
     <sheet name="Mise - fáze" sheetId="3" r:id="rId4"/>
     <sheet name="Frakce" sheetId="8" r:id="rId5"/>
     <sheet name="Hráč" sheetId="5" r:id="rId6"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="244">
   <si>
     <t>ID</t>
   </si>
@@ -654,6 +654,126 @@
   </si>
   <si>
     <t>Opilý poník je hlučná hospoda v centru města. Její stěny jsou z hrubě opracovaného kamene a střecha je pokrytá slámou. Uvnitř je hospoda hlučná a bujará, podél jedné stěny se táhne velký bar a na druhé straně doutná krb. Barmani jsou nevrlí a rychle obsluhují, zatímco hosté jsou neurvalá parta, která křičí a směje se za zvuků řinčení sklenic a vrzání prken. Jídelní lístek v restauraci The Drunken Pony se skládá převážně z vydatných dušených jídel a masa, které se zapíjejí velkými hrnky pěnivého piva. Krčma je oblíbeným místem cestovatelů, obchodníků i místních obyvatel, kteří sem chodí popíjet, vyprávět si příběhy a sdílet kamarádství na cestách.</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>drugs</t>
+  </si>
+  <si>
+    <t>misc</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>weapon</t>
+  </si>
+  <si>
+    <t>usage</t>
+  </si>
+  <si>
+    <t>Pivo Horal</t>
+  </si>
+  <si>
+    <t>Černá břečka</t>
+  </si>
+  <si>
+    <t>Rybí voda</t>
+  </si>
+  <si>
+    <t>Chleba</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>consume</t>
+  </si>
+  <si>
+    <t>equip</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>shop,food</t>
+  </si>
+  <si>
+    <t>shop,weapon</t>
+  </si>
+  <si>
+    <t>shop,misc</t>
+  </si>
+  <si>
+    <t>shop,drugs</t>
+  </si>
+  <si>
+    <t>free</t>
+  </si>
+  <si>
+    <t>Tajné heslo</t>
+  </si>
+  <si>
+    <t>Tajná formulka</t>
+  </si>
+  <si>
+    <t>V ruce držíš malý ušmudlaný papírek, který se vlivem času skoro rozpadl. Je na něm napsáno pár slůvek: Ty mě zub, já tobě oko. Ty mě oko já tobě duši.</t>
+  </si>
+  <si>
+    <t>Tento zažloutlý cár papíru podivně zapáchá rybinou. Navíc na něj někdo roztřesenou rukou napsal: Smrad nebo smrt? Raději oboje.</t>
+  </si>
+  <si>
+    <t>Trochu ztvrdlý, ale jinak poctivý pecen.</t>
+  </si>
+  <si>
+    <t>Původně sis myslel, že jde o polévku, ale opravdu je to nejspíš jen mořská voda, která možná někdy rybu viděla.</t>
+  </si>
+  <si>
+    <t>Je to černé a alkoholické. Co víc potřebuje člověk vědět.</t>
+  </si>
+  <si>
+    <t>Pivo místního sládka, asi jediná věc ve měste, ze které se člověku neudělá špatně.</t>
+  </si>
+  <si>
+    <t>Krátký ale ostrý. Neřízni se</t>
+  </si>
+  <si>
+    <t>I tahle ryba kdysi nejspíš měla rodinu, ale zbraň taky dobrá.</t>
+  </si>
+  <si>
+    <t>I když kód hlídky káže, že by zaměstnanci měli udržovat svoje zbraně čisté, tak původní majitel se toho moc nedržel. Kovovými plátky vyztužené dřevo totiž pokrývají zaschlé cákance krve.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je tohle osud, který pro nás bohové přichystali? 13 ohařů, jež budou zasévat nekonečné bolesti. </t>
+  </si>
+  <si>
+    <t>Je to smutné pomyšlení, že kdysi byla používaná na vyvrhávání obětin a  tu s ní teď jen tak máváš.</t>
+  </si>
+  <si>
+    <t>Sirky značky Dobrého nepálí</t>
+  </si>
+  <si>
+    <t>Bylo bíle. Teď není. Bývalo čisté. Teď je potřísněné. Čím? Lepší nevědět, ale hlavně k němu nečichej.</t>
+  </si>
+  <si>
+    <t>Nejpopulárnější droga na trhu, ale nebezpečně návyková. Pokud teda slovo návyková používáte ve smyslu: prodám sebe i celou svou rodinu do otroctví, abych si mohl dovolit ještě jednu dávku.</t>
+  </si>
+  <si>
+    <t>Toto jmění ve formě prášku má větší cenu než místní hrad a životy všech lidí ve městě dohromady.</t>
+  </si>
+  <si>
+    <t>item:15</t>
+  </si>
+  <si>
+    <t>item:14</t>
+  </si>
+  <si>
+    <t>item:6</t>
+  </si>
+  <si>
+    <t>access</t>
   </si>
 </sst>
 </file>
@@ -690,7 +810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -703,9 +823,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1020,11 +1137,529 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78C4A7C-2711-4806-8FFC-B45798D03982}">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2">
+        <v>-2</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>2000</v>
+      </c>
+      <c r="H2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>500</v>
+      </c>
+      <c r="H3" t="s">
+        <v>205</v>
+      </c>
+      <c r="I3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>50</v>
+      </c>
+      <c r="H4" t="s">
+        <v>205</v>
+      </c>
+      <c r="I4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>206</v>
+      </c>
+      <c r="I5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" t="s">
+        <v>235</v>
+      </c>
+      <c r="D6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>40</v>
+      </c>
+      <c r="H6" t="s">
+        <v>208</v>
+      </c>
+      <c r="I6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7">
+        <v>-1</v>
+      </c>
+      <c r="F7">
+        <v>-1</v>
+      </c>
+      <c r="G7">
+        <v>60</v>
+      </c>
+      <c r="H7" t="s">
+        <v>207</v>
+      </c>
+      <c r="I7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" t="s">
+        <v>237</v>
+      </c>
+      <c r="D8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8">
+        <v>-1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>69</v>
+      </c>
+      <c r="H8" t="s">
+        <v>207</v>
+      </c>
+      <c r="I8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9">
+        <v>-1</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>35</v>
+      </c>
+      <c r="H9" t="s">
+        <v>208</v>
+      </c>
+      <c r="I9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D10" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10">
+        <v>-1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>208</v>
+      </c>
+      <c r="I10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C11" t="s">
+        <v>231</v>
+      </c>
+      <c r="D11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11">
+        <v>-1</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>20</v>
+      </c>
+      <c r="H11" t="s">
+        <v>208</v>
+      </c>
+      <c r="I11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" t="s">
+        <v>230</v>
+      </c>
+      <c r="D12" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12">
+        <v>-1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>214</v>
+      </c>
+      <c r="I12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" t="s">
+        <v>229</v>
+      </c>
+      <c r="D13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>-1</v>
+      </c>
+      <c r="G13">
+        <v>15</v>
+      </c>
+      <c r="H13" t="s">
+        <v>214</v>
+      </c>
+      <c r="I13" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>15</v>
+      </c>
+      <c r="H14" t="s">
+        <v>214</v>
+      </c>
+      <c r="I14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>213</v>
+      </c>
+      <c r="C15" t="s">
+        <v>227</v>
+      </c>
+      <c r="D15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>10</v>
+      </c>
+      <c r="H15" t="s">
+        <v>214</v>
+      </c>
+      <c r="I15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>223</v>
+      </c>
+      <c r="C16" t="s">
+        <v>226</v>
+      </c>
+      <c r="D16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>100</v>
+      </c>
+      <c r="H16" t="s">
+        <v>207</v>
+      </c>
+      <c r="I16" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>224</v>
+      </c>
+      <c r="C17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+      <c r="H17" t="s">
+        <v>207</v>
+      </c>
+      <c r="I17" t="s">
+        <v>217</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9C1193-21D4-4077-9037-2F33601C62B1}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,7 +1668,8 @@
     <col min="2" max="2" width="31.85546875" customWidth="1"/>
     <col min="3" max="3" width="39.7109375" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1052,7 +1688,9 @@
       <c r="E1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>243</v>
+      </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1070,8 +1708,12 @@
       <c r="D2" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1090,7 +1732,9 @@
         <v>177</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1105,11 +1749,13 @@
       <c r="C4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="1" t="s">
         <v>172</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -1124,11 +1770,15 @@
       <c r="C5" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1143,11 +1793,13 @@
       <c r="C6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1162,11 +1814,13 @@
       <c r="C7" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="1" t="s">
         <v>182</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1181,11 +1835,13 @@
       <c r="C8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="1" t="s">
         <v>162</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1200,11 +1856,13 @@
       <c r="C9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="1" t="s">
         <v>184</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1219,11 +1877,13 @@
       <c r="C10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="1" t="s">
         <v>191</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1238,11 +1898,13 @@
       <c r="C11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="1" t="s">
         <v>165</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1257,11 +1919,13 @@
       <c r="C12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="1" t="s">
         <v>188</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1276,11 +1940,13 @@
       <c r="C13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="1" t="s">
         <v>171</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1295,11 +1961,13 @@
       <c r="C14" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="1" t="s">
         <v>164</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1314,11 +1982,15 @@
       <c r="C15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1333,11 +2005,13 @@
       <c r="C16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="1" t="s">
         <v>180</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1352,11 +2026,13 @@
       <c r="C17" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="1" t="s">
         <v>170</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -1371,11 +2047,15 @@
       <c r="C18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1390,11 +2070,13 @@
       <c r="C19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="1" t="s">
         <v>190</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -1409,11 +2091,13 @@
       <c r="C20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="1" t="s">
         <v>167</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -1428,11 +2112,13 @@
       <c r="C21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="1" t="s">
         <v>187</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -1447,11 +2133,13 @@
       <c r="C22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="1" t="s">
         <v>178</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1466,11 +2154,13 @@
       <c r="C23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="1" t="s">
         <v>186</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -1485,11 +2175,13 @@
       <c r="C24" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="1" t="s">
         <v>166</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -1504,11 +2196,13 @@
       <c r="C25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="1" t="s">
         <v>185</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -1523,11 +2217,13 @@
       <c r="C26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="1" t="s">
         <v>193</v>
       </c>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -1542,11 +2238,13 @@
       <c r="C27" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="1" t="s">
         <v>176</v>
       </c>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="F27" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -1561,11 +2259,13 @@
       <c r="C28" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="1" t="s">
         <v>174</v>
       </c>
       <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -1580,11 +2280,13 @@
       <c r="C29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="1" t="s">
         <v>183</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -1599,11 +2301,15 @@
       <c r="C30" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="E30" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -1618,11 +2324,13 @@
       <c r="C31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="1" t="s">
         <v>189</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="F31" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -1637,11 +2345,13 @@
       <c r="C32" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+      <c r="F32" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -1656,11 +2366,13 @@
       <c r="C33" s="1">
         <v>29</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="1" t="s">
         <v>179</v>
       </c>
       <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+      <c r="F33" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -1675,8 +2387,12 @@
       <c r="C34" s="1">
         <v>27</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="2" t="s">
         <v>194</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="1" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1689,8 +2405,12 @@
       <c r="C35" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="2" t="s">
         <v>195</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="1" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1703,8 +2423,12 @@
       <c r="C36" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="2" t="s">
         <v>196</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="1" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1717,8 +2441,12 @@
       <c r="C37" s="1">
         <v>12</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="2" t="s">
         <v>197</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="1" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1731,8 +2459,14 @@
       <c r="C38" s="1">
         <v>5</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="2" t="s">
         <v>198</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -1745,8 +2479,14 @@
       <c r="C39" s="1">
         <v>3</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="2" t="s">
         <v>199</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -1759,8 +2499,12 @@
       <c r="C40" s="1">
         <v>28</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="2" t="s">
         <v>200</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="1" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1773,8 +2517,12 @@
       <c r="C41" s="1">
         <v>15</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="2" t="s">
         <v>201</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="1" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -1786,7 +2534,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE42307A-777D-49E3-9DBB-1C926DF7AB9F}">
   <dimension ref="A1:I36"/>
   <sheetViews>
@@ -1860,11 +2608,11 @@
       </c>
       <c r="H2">
         <f ca="1">RANDBETWEEN(1,5-G2)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I2">
         <f ca="1">RANDBETWEEN(0,20)</f>
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1888,15 +2636,15 @@
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G36" ca="1" si="0">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H36" ca="1" si="1">RANDBETWEEN(1,5-G3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I36" ca="1" si="2">RANDBETWEEN(0,20)</f>
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1924,11 +2672,11 @@
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1952,15 +2700,15 @@
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1984,15 +2732,15 @@
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2016,15 +2764,15 @@
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2048,7 +2796,7 @@
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="1"/>
@@ -2056,7 +2804,7 @@
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2080,15 +2828,15 @@
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2112,15 +2860,15 @@
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2144,7 +2892,7 @@
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
@@ -2152,7 +2900,7 @@
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2176,15 +2924,15 @@
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2208,7 +2956,7 @@
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="1"/>
@@ -2216,7 +2964,7 @@
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2240,7 +2988,7 @@
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="1"/>
@@ -2248,7 +2996,7 @@
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2272,15 +3020,15 @@
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2308,11 +3056,11 @@
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2336,15 +3084,15 @@
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2376,7 +3124,7 @@
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2400,15 +3148,15 @@
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2432,15 +3180,15 @@
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2464,15 +3212,15 @@
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2496,15 +3244,15 @@
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2528,15 +3276,15 @@
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2560,15 +3308,15 @@
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2592,7 +3340,7 @@
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
@@ -2600,7 +3348,7 @@
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2624,15 +3372,15 @@
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2656,15 +3404,15 @@
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2696,7 +3444,7 @@
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2724,11 +3472,11 @@
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2752,7 +3500,7 @@
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
@@ -2760,7 +3508,7 @@
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2784,15 +3532,15 @@
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2816,7 +3564,7 @@
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="1"/>
@@ -2824,7 +3572,7 @@
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2856,7 +3604,7 @@
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2880,7 +3628,7 @@
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="1"/>
@@ -2888,7 +3636,7 @@
       </c>
       <c r="I34">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2920,7 +3668,7 @@
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2952,250 +3700,7 @@
       </c>
       <c r="I36">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78C4A7C-2711-4806-8FFC-B45798D03982}">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2">
-        <v>-2</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3">
-        <v>-1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D7">
-        <v>-1</v>
-      </c>
-      <c r="E7">
-        <v>-1</v>
-      </c>
-      <c r="F7">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>144</v>
-      </c>
-      <c r="C8" t="s">
-        <v>138</v>
-      </c>
-      <c r="D8">
-        <v>-1</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9">
-        <v>-1</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
         <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>149</v>
-      </c>
-      <c r="C10" t="s">
-        <v>138</v>
-      </c>
-      <c r="D10">
-        <v>-1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>150</v>
-      </c>
-      <c r="C11" t="s">
-        <v>138</v>
-      </c>
-      <c r="D11">
-        <v>-1</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added basic telegram controls
</commit_message>
<xml_diff>
--- a/zzz_other/tables.xlsx
+++ b/zzz_other/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Filip\škola\!!!_MATRIP\DnD\zzz_other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5709D51D-4D67-4B79-A93A-B401D594D5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC80750-DE73-4E33-8A54-F1B932A65E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{75D15189-BFBB-4142-B930-759327EB73F3}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="245">
   <si>
     <t>ID</t>
   </si>
@@ -698,15 +698,6 @@
     <t>shop,food</t>
   </si>
   <si>
-    <t>shop,weapon</t>
-  </si>
-  <si>
-    <t>shop,misc</t>
-  </si>
-  <si>
-    <t>shop,drugs</t>
-  </si>
-  <si>
     <t>free</t>
   </si>
   <si>
@@ -774,6 +765,18 @@
   </si>
   <si>
     <t>33;14;25;0</t>
+  </si>
+  <si>
+    <t>shop:food</t>
+  </si>
+  <si>
+    <t>shop:misc</t>
+  </si>
+  <si>
+    <t>shop:drugs</t>
+  </si>
+  <si>
+    <t>shop:weapon</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1196,7 @@
         <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D2" t="s">
         <v>73</v>
@@ -1222,7 +1225,7 @@
         <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D3" t="s">
         <v>73</v>
@@ -1251,7 +1254,7 @@
         <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D4" t="s">
         <v>73</v>
@@ -1280,7 +1283,7 @@
         <v>138</v>
       </c>
       <c r="C5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D5" t="s">
         <v>137</v>
@@ -1309,7 +1312,7 @@
         <v>139</v>
       </c>
       <c r="C6" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D6" t="s">
         <v>137</v>
@@ -1338,7 +1341,7 @@
         <v>140</v>
       </c>
       <c r="C7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D7" t="s">
         <v>137</v>
@@ -1367,7 +1370,7 @@
         <v>143</v>
       </c>
       <c r="C8" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D8" t="s">
         <v>137</v>
@@ -1396,7 +1399,7 @@
         <v>144</v>
       </c>
       <c r="C9" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D9" t="s">
         <v>73</v>
@@ -1425,7 +1428,7 @@
         <v>148</v>
       </c>
       <c r="C10" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D10" t="s">
         <v>137</v>
@@ -1454,7 +1457,7 @@
         <v>149</v>
       </c>
       <c r="C11" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D11" t="s">
         <v>137</v>
@@ -1483,7 +1486,7 @@
         <v>209</v>
       </c>
       <c r="C12" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D12" t="s">
         <v>137</v>
@@ -1512,7 +1515,7 @@
         <v>210</v>
       </c>
       <c r="C13" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D13" t="s">
         <v>137</v>
@@ -1541,7 +1544,7 @@
         <v>211</v>
       </c>
       <c r="C14" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D14" t="s">
         <v>137</v>
@@ -1570,7 +1573,7 @@
         <v>212</v>
       </c>
       <c r="C15" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D15" t="s">
         <v>137</v>
@@ -1596,10 +1599,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>219</v>
+      </c>
+      <c r="C16" t="s">
         <v>222</v>
-      </c>
-      <c r="C16" t="s">
-        <v>225</v>
       </c>
       <c r="D16" t="s">
         <v>73</v>
@@ -1625,10 +1628,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C17" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D17" t="s">
         <v>73</v>
@@ -1659,7 +1662,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1689,7 +1692,7 @@
         <v>201</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1709,10 +1712,10 @@
         <v>202</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -1733,7 +1736,7 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1754,7 +1757,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1777,7 +1780,7 @@
         <v>217</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1798,7 +1801,7 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1819,7 +1822,7 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1840,7 +1843,7 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1861,7 +1864,7 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1882,7 +1885,7 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1903,7 +1906,7 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1924,7 +1927,7 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1945,7 +1948,7 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1966,7 +1969,7 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1986,10 +1989,10 @@
         <v>167</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>219</v>
+        <v>242</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -2010,7 +2013,7 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -2031,7 +2034,7 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -2051,10 +2054,10 @@
         <v>191</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>220</v>
+        <v>243</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -2075,7 +2078,7 @@
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -2096,7 +2099,7 @@
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -2117,7 +2120,7 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -2131,14 +2134,14 @@
         <v>15</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>177</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -2159,7 +2162,7 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -2180,7 +2183,7 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -2201,7 +2204,7 @@
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -2222,7 +2225,7 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -2243,7 +2246,7 @@
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -2264,7 +2267,7 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -2285,7 +2288,7 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -2305,10 +2308,10 @@
         <v>174</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -2329,7 +2332,7 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -2350,7 +2353,7 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -2371,7 +2374,7 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -2392,7 +2395,7 @@
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2410,7 +2413,7 @@
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2428,7 +2431,7 @@
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2446,7 +2449,7 @@
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2463,10 +2466,10 @@
         <v>197</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>220</v>
+        <v>243</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2483,10 +2486,10 @@
         <v>198</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>220</v>
+        <v>243</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2504,7 +2507,7 @@
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2522,7 +2525,7 @@
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -2604,15 +2607,15 @@
       </c>
       <c r="G2">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <f ca="1">RANDBETWEEN(1,5-G2)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I2">
         <f ca="1">RANDBETWEEN(0,20)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2636,15 +2639,15 @@
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G36" ca="1" si="0">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H36" ca="1" si="1">RANDBETWEEN(1,5-G3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I36" ca="1" si="2">RANDBETWEEN(0,20)</f>
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2668,11 +2671,11 @@
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="2"/>
@@ -2700,7 +2703,7 @@
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
@@ -2708,7 +2711,7 @@
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2732,15 +2735,15 @@
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2764,15 +2767,15 @@
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2804,7 +2807,7 @@
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2828,15 +2831,15 @@
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2864,11 +2867,11 @@
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2892,15 +2895,15 @@
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2928,11 +2931,11 @@
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2956,15 +2959,15 @@
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2992,11 +2995,11 @@
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3020,15 +3023,15 @@
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3052,7 +3055,7 @@
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="1"/>
@@ -3060,7 +3063,7 @@
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -3092,7 +3095,7 @@
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -3116,15 +3119,15 @@
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -3148,7 +3151,7 @@
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
@@ -3156,7 +3159,7 @@
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -3180,15 +3183,15 @@
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -3212,7 +3215,7 @@
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
@@ -3220,7 +3223,7 @@
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -3244,15 +3247,15 @@
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -3280,11 +3283,11 @@
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3308,15 +3311,15 @@
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -3340,11 +3343,11 @@
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="2"/>
@@ -3380,7 +3383,7 @@
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -3408,11 +3411,11 @@
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -3436,15 +3439,15 @@
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -3472,11 +3475,11 @@
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -3504,11 +3507,11 @@
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -3532,7 +3535,7 @@
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="1"/>
@@ -3540,7 +3543,7 @@
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -3564,15 +3567,15 @@
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3596,15 +3599,15 @@
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3636,7 +3639,7 @@
       </c>
       <c r="I34">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -3660,15 +3663,15 @@
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -3692,15 +3695,15 @@
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I36">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added hopefully working inventory support to telegram
</commit_message>
<xml_diff>
--- a/zzz_other/tables.xlsx
+++ b/zzz_other/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Filip\škola\!!!_MATRIP\DnD\zzz_other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5968C5-1DE2-4DF1-B50D-73343153544F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C830230-E874-409B-9389-3589BC08C0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{75D15189-BFBB-4142-B930-759327EB73F3}"/>
+    <workbookView xWindow="28680" yWindow="-6615" windowWidth="16440" windowHeight="28440" activeTab="2" xr2:uid="{75D15189-BFBB-4142-B930-759327EB73F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Předměty" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="246">
   <si>
     <t>ID</t>
   </si>
@@ -275,9 +275,6 @@
     <t>1;2;11;36</t>
   </si>
   <si>
-    <t>quest_line_ID</t>
-  </si>
-  <si>
     <t>Zásilka šňupce</t>
   </si>
   <si>
@@ -777,6 +774,12 @@
   </si>
   <si>
     <t>Cedrová ulice je plná domů obložených cedrovým dřevem, jejichž verandy a balkony poskytují úkryt před zapadajícím sluncem.</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>Barman Brčko</t>
   </si>
 </sst>
 </file>
@@ -1141,25 +1144,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78C4A7C-2711-4806-8FFC-B45798D03982}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="3" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1167,489 +1172,540 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>162</v>
+        <v>72</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="E1" t="s">
         <v>141</v>
       </c>
       <c r="F1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G1" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="H1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I1" t="s">
+        <v>244</v>
+      </c>
+      <c r="J1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2">
+        <v>-2</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>2000</v>
+      </c>
+      <c r="G2" t="s">
         <v>202</v>
       </c>
-      <c r="I1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="H2" t="s">
+        <v>214</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>78</v>
       </c>
-      <c r="C2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>73</v>
       </c>
-      <c r="E2">
-        <v>-2</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>2000</v>
-      </c>
-      <c r="H2" t="s">
-        <v>203</v>
-      </c>
-      <c r="I2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" t="s">
-        <v>233</v>
-      </c>
-      <c r="D3" t="s">
-        <v>73</v>
+      <c r="D3">
+        <v>-1</v>
       </c>
       <c r="E3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
         <v>500</v>
       </c>
+      <c r="G3" t="s">
+        <v>202</v>
+      </c>
       <c r="H3" t="s">
-        <v>203</v>
-      </c>
-      <c r="I3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
-      </c>
-      <c r="D4" t="s">
         <v>73</v>
       </c>
+      <c r="D4">
+        <v>-3</v>
+      </c>
       <c r="E4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
         <v>50</v>
       </c>
+      <c r="G4" t="s">
+        <v>202</v>
+      </c>
       <c r="H4" t="s">
-        <v>203</v>
-      </c>
-      <c r="I4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
-        <v>231</v>
-      </c>
-      <c r="D5" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
         <v>2</v>
       </c>
+      <c r="G5" t="s">
+        <v>203</v>
+      </c>
       <c r="H5" t="s">
-        <v>204</v>
-      </c>
-      <c r="I5" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C6" t="s">
-        <v>230</v>
-      </c>
-      <c r="D6" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6">
         <v>40</v>
       </c>
+      <c r="G6" t="s">
+        <v>205</v>
+      </c>
       <c r="H6" t="s">
-        <v>206</v>
-      </c>
-      <c r="I6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C7" t="s">
-        <v>229</v>
-      </c>
-      <c r="D7" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="D7">
+        <v>-1</v>
       </c>
       <c r="E7">
         <v>-1</v>
       </c>
       <c r="F7">
-        <v>-1</v>
-      </c>
-      <c r="G7">
         <v>60</v>
       </c>
+      <c r="G7" t="s">
+        <v>204</v>
+      </c>
       <c r="H7" t="s">
-        <v>205</v>
-      </c>
-      <c r="I7" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C8" t="s">
-        <v>232</v>
-      </c>
-      <c r="D8" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="D8">
+        <v>-1</v>
       </c>
       <c r="E8">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
         <v>69</v>
       </c>
+      <c r="G8" t="s">
+        <v>204</v>
+      </c>
       <c r="H8" t="s">
-        <v>205</v>
-      </c>
-      <c r="I8" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C9" t="s">
-        <v>228</v>
-      </c>
-      <c r="D9" t="s">
         <v>73</v>
       </c>
+      <c r="D9">
+        <v>-1</v>
+      </c>
       <c r="E9">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9">
         <v>35</v>
       </c>
+      <c r="G9" t="s">
+        <v>205</v>
+      </c>
       <c r="H9" t="s">
-        <v>206</v>
-      </c>
-      <c r="I9" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C10" t="s">
-        <v>227</v>
-      </c>
-      <c r="D10" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="D10">
+        <v>-1</v>
       </c>
       <c r="E10">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
         <v>15</v>
       </c>
+      <c r="G10" t="s">
+        <v>205</v>
+      </c>
       <c r="H10" t="s">
-        <v>206</v>
-      </c>
-      <c r="I10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C11" t="s">
-        <v>226</v>
-      </c>
-      <c r="D11" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="D11">
+        <v>-1</v>
       </c>
       <c r="E11">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F11">
-        <v>2</v>
-      </c>
-      <c r="G11">
         <v>20</v>
       </c>
+      <c r="G11" t="s">
+        <v>205</v>
+      </c>
       <c r="H11" t="s">
-        <v>206</v>
-      </c>
-      <c r="I11" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C12" t="s">
-        <v>225</v>
-      </c>
-      <c r="D12" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="D12">
+        <v>-1</v>
       </c>
       <c r="E12">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
         <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>211</v>
       </c>
       <c r="H12" t="s">
         <v>212</v>
       </c>
-      <c r="I12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="J12" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C13" t="s">
-        <v>224</v>
-      </c>
-      <c r="D13" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F13">
-        <v>-1</v>
-      </c>
-      <c r="G13">
         <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>211</v>
       </c>
       <c r="H13" t="s">
         <v>212</v>
       </c>
-      <c r="I13" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>12</v>
+      </c>
+      <c r="J13" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C14" t="s">
-        <v>223</v>
-      </c>
-      <c r="D14" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
         <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>211</v>
       </c>
       <c r="H14" t="s">
         <v>212</v>
       </c>
-      <c r="I14" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>15</v>
+      </c>
+      <c r="J14" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>210</v>
+      </c>
+      <c r="C15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
         <v>211</v>
-      </c>
-      <c r="C15" t="s">
-        <v>222</v>
-      </c>
-      <c r="D15" t="s">
-        <v>137</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>10</v>
       </c>
       <c r="H15" t="s">
         <v>212</v>
       </c>
-      <c r="I15" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>12</v>
+      </c>
+      <c r="J15" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C16" t="s">
-        <v>221</v>
-      </c>
-      <c r="D16" t="s">
         <v>73</v>
       </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
         <v>100</v>
       </c>
+      <c r="G16" t="s">
+        <v>204</v>
+      </c>
       <c r="H16" t="s">
-        <v>205</v>
-      </c>
-      <c r="I16" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>100</v>
+      </c>
+      <c r="G17" t="s">
+        <v>204</v>
+      </c>
+      <c r="H17" t="s">
+        <v>214</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
         <v>219</v>
-      </c>
-      <c r="C17" t="s">
-        <v>220</v>
-      </c>
-      <c r="D17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>100</v>
-      </c>
-      <c r="H17" t="s">
-        <v>205</v>
-      </c>
-      <c r="I17" t="s">
-        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -1661,7 +1717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9C1193-21D4-4077-9037-2F33601C62B1}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -1686,13 +1742,13 @@
         <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1709,13 +1765,13 @@
         <v>20</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -1732,11 +1788,11 @@
         <v>34</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1753,11 +1809,11 @@
         <v>52</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1771,16 +1827,16 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1797,11 +1853,11 @@
         <v>51</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1818,11 +1874,11 @@
         <v>76</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1839,11 +1895,11 @@
         <v>55</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1860,11 +1916,11 @@
         <v>54</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1881,11 +1937,11 @@
         <v>48</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1902,11 +1958,11 @@
         <v>56</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1923,11 +1979,11 @@
         <v>50</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1944,11 +2000,11 @@
         <v>58</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1965,11 +2021,11 @@
         <v>75</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1986,13 +2042,13 @@
         <v>38</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -2009,11 +2065,11 @@
         <v>37</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -2027,14 +2083,14 @@
         <v>12</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -2051,13 +2107,13 @@
         <v>36</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -2074,11 +2130,11 @@
         <v>47</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -2095,11 +2151,11 @@
         <v>61</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -2116,11 +2172,11 @@
         <v>53</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -2134,14 +2190,14 @@
         <v>15</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -2158,11 +2214,11 @@
         <v>45</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -2179,11 +2235,11 @@
         <v>60</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -2200,11 +2256,11 @@
         <v>41</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -2221,11 +2277,11 @@
         <v>44</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -2242,11 +2298,11 @@
         <v>39</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -2263,11 +2319,11 @@
         <v>35</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -2284,11 +2340,11 @@
         <v>40</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -2302,16 +2358,16 @@
         <v>23</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -2328,11 +2384,11 @@
         <v>46</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -2349,11 +2405,11 @@
         <v>59</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -2370,11 +2426,11 @@
         <v>29</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -2391,11 +2447,11 @@
         <v>27</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2409,11 +2465,11 @@
         <v>49</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2427,11 +2483,11 @@
         <v>57</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2445,11 +2501,11 @@
         <v>12</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2463,13 +2519,13 @@
         <v>5</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2477,19 +2533,19 @@
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C39" s="1">
         <v>3</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2497,17 +2553,17 @@
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C40" s="1">
         <v>28</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2515,17 +2571,17 @@
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C41" s="1">
         <v>15</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2539,25 +2595,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE42307A-777D-49E3-9DBB-1C926DF7AB9F}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.140625" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2565,28 +2620,25 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F1" t="s">
-        <v>64</v>
+        <v>145</v>
       </c>
       <c r="G1" t="s">
         <v>146</v>
       </c>
       <c r="H1" t="s">
-        <v>147</v>
-      </c>
-      <c r="I1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2597,1113 +2649,1037 @@
         <v>6</v>
       </c>
       <c r="D2">
+        <v>32</v>
+      </c>
+      <c r="E2">
         <v>-1</v>
       </c>
-      <c r="E2">
-        <v>32</v>
-      </c>
       <c r="F2">
-        <v>-1</v>
+        <f ca="1">RANDBETWEEN(1,4)</f>
+        <v>1</v>
       </c>
       <c r="G2">
-        <f ca="1">RANDBETWEEN(1,4)</f>
+        <f ca="1">RANDBETWEEN(1,5-F2)</f>
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <f ca="1">RANDBETWEEN(10,70)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>35</v>
+      </c>
+      <c r="E3">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F37" ca="1" si="0">RANDBETWEEN(1,4)</f>
         <v>4</v>
       </c>
-      <c r="H2">
-        <f ca="1">RANDBETWEEN(1,5-G2)</f>
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <f ca="1">RANDBETWEEN(0,20)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>-1</v>
-      </c>
-      <c r="E3">
-        <v>35</v>
-      </c>
-      <c r="F3">
-        <v>14</v>
-      </c>
       <c r="G3">
-        <f t="shared" ref="G3:G36" ca="1" si="0">RANDBETWEEN(1,4)</f>
+        <f t="shared" ref="G3:G37" ca="1" si="1">RANDBETWEEN(1,5-F3)</f>
         <v>1</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H36" ca="1" si="1">RANDBETWEEN(1,5-G3)</f>
-        <v>3</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I36" ca="1" si="2">RANDBETWEEN(0,20)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H3:H36" ca="1" si="2">RANDBETWEEN(10,70)</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>-1</v>
+        <v>35</v>
       </c>
       <c r="E4">
         <v>35</v>
       </c>
       <c r="F4">
-        <v>35</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
       </c>
       <c r="G4">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="H4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I4">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>-1</v>
+        <v>35</v>
       </c>
       <c r="E5">
         <v>35</v>
       </c>
       <c r="F5">
-        <v>35</v>
-      </c>
-      <c r="G5">
         <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
+      <c r="G5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
       <c r="H5">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I5">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>-1</v>
+        <v>33</v>
       </c>
       <c r="E6">
         <v>33</v>
       </c>
       <c r="F6">
-        <v>33</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
       </c>
       <c r="G6">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ca="1" si="2"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>34</v>
+      </c>
+      <c r="E7">
+        <v>34</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ca="1" si="2"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <v>-1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ca="1" si="2"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ca="1" si="2"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>13</v>
+      </c>
+      <c r="E10">
+        <v>-1</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ca="1" si="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>23</v>
+      </c>
+      <c r="E11">
+        <v>23</v>
+      </c>
+      <c r="F11">
         <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="H6">
+      <c r="G11">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
-      <c r="I6">
+      <c r="H11">
         <f t="shared" ca="1" si="2"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>23</v>
+      </c>
+      <c r="E12">
+        <v>23</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ca="1" si="2"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>37</v>
+      </c>
+      <c r="E13">
+        <v>37</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>-1</v>
-      </c>
-      <c r="E7">
-        <v>34</v>
-      </c>
-      <c r="F7">
-        <v>34</v>
-      </c>
-      <c r="G7">
+      <c r="H13">
+        <f t="shared" ca="1" si="2"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>37</v>
+      </c>
+      <c r="E14">
+        <v>37</v>
+      </c>
+      <c r="F14">
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7">
+      <c r="G14">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="H14">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>-1</v>
-      </c>
-      <c r="E8">
-        <v>17</v>
-      </c>
-      <c r="F8">
-        <v>-1</v>
-      </c>
-      <c r="G8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>37</v>
+      </c>
+      <c r="E15">
+        <v>37</v>
+      </c>
+      <c r="F15">
         <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
-      <c r="H8">
+      <c r="G15">
         <f t="shared" ca="1" si="1"/>
         <v>2</v>
       </c>
-      <c r="I8">
+      <c r="H15">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>105</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>-1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>37</v>
+      </c>
+      <c r="E16">
+        <v>37</v>
+      </c>
+      <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="G16">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
-      <c r="I9">
+      <c r="H16">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>-1</v>
-      </c>
-      <c r="E10">
-        <v>13</v>
-      </c>
-      <c r="F10">
-        <v>-1</v>
-      </c>
-      <c r="G10">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>37</v>
+      </c>
+      <c r="E17">
+        <v>37</v>
+      </c>
+      <c r="F17">
         <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="H10">
+      <c r="G17">
         <f t="shared" ca="1" si="1"/>
         <v>2</v>
       </c>
-      <c r="I10">
+      <c r="H17">
         <f t="shared" ca="1" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11">
-        <v>-1</v>
-      </c>
-      <c r="E11">
-        <v>23</v>
-      </c>
-      <c r="F11">
-        <v>23</v>
-      </c>
-      <c r="G11">
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>38</v>
+      </c>
+      <c r="E18">
+        <v>38</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ca="1" si="2"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>38</v>
+      </c>
+      <c r="E19">
+        <v>38</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <f t="shared" ca="1" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>38</v>
+      </c>
+      <c r="E20">
+        <v>38</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ca="1" si="2"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>38</v>
+      </c>
+      <c r="E21">
+        <v>38</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ca="1" si="2"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>38</v>
+      </c>
+      <c r="E22">
+        <v>38</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <f t="shared" ca="1" si="2"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>39</v>
+      </c>
+      <c r="E23">
+        <v>39</v>
+      </c>
+      <c r="F23">
         <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="H11">
+      <c r="G23">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
-      <c r="I11">
+      <c r="H23">
+        <f t="shared" ca="1" si="2"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>39</v>
+      </c>
+      <c r="E24">
+        <v>39</v>
+      </c>
+      <c r="F24">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <f t="shared" ca="1" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>39</v>
+      </c>
+      <c r="E25">
+        <v>39</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ca="1" si="2"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>39</v>
+      </c>
+      <c r="E26">
+        <v>39</v>
+      </c>
+      <c r="F26">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <f t="shared" ca="1" si="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>39</v>
+      </c>
+      <c r="E27">
+        <v>39</v>
+      </c>
+      <c r="F27">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <f t="shared" ca="1" si="2"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>39</v>
+      </c>
+      <c r="E28">
+        <v>39</v>
+      </c>
+      <c r="F28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <f t="shared" ca="1" si="2"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>7</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <f t="shared" ca="1" si="2"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>7</v>
+      </c>
+      <c r="E30">
+        <v>7</v>
+      </c>
+      <c r="F30">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H30">
         <f t="shared" ca="1" si="2"/>
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12">
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <v>-1</v>
-      </c>
-      <c r="E12">
-        <v>23</v>
-      </c>
-      <c r="F12">
-        <v>23</v>
-      </c>
-      <c r="G12">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>153</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>7</v>
+      </c>
+      <c r="E31">
+        <v>7</v>
+      </c>
+      <c r="F31">
         <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="H12">
+      <c r="G31">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <f t="shared" ca="1" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>154</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G32">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <f t="shared" ca="1" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G33">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H33">
+        <f t="shared" ca="1" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>156</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>19</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G34">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <f t="shared" ca="1" si="2"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>157</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>20</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <f t="shared" ca="1" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>158</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G36">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <f t="shared" ca="1" si="2"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>245</v>
+      </c>
+      <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G37">
         <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
-      <c r="I12">
-        <f t="shared" ca="1" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>-1</v>
-      </c>
-      <c r="E13">
-        <v>37</v>
-      </c>
-      <c r="F13">
-        <v>37</v>
-      </c>
-      <c r="G13">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H13">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>-1</v>
-      </c>
-      <c r="E14">
-        <v>37</v>
-      </c>
-      <c r="F14">
-        <v>37</v>
-      </c>
-      <c r="G14">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="I14">
-        <f t="shared" ca="1" si="2"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>111</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>-1</v>
-      </c>
-      <c r="E15">
-        <v>37</v>
-      </c>
-      <c r="F15">
-        <v>37</v>
-      </c>
-      <c r="G15">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H15">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <f t="shared" ca="1" si="2"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>112</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>-1</v>
-      </c>
-      <c r="E16">
-        <v>37</v>
-      </c>
-      <c r="F16">
-        <v>37</v>
-      </c>
-      <c r="G16">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H16">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <f t="shared" ca="1" si="2"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>-1</v>
-      </c>
-      <c r="E17">
-        <v>37</v>
-      </c>
-      <c r="F17">
-        <v>37</v>
-      </c>
-      <c r="G17">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H17">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="H37">
+        <f ca="1">RANDBETWEEN(10,70)</f>
         <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>114</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18">
-        <v>-1</v>
-      </c>
-      <c r="E18">
-        <v>38</v>
-      </c>
-      <c r="F18">
-        <v>38</v>
-      </c>
-      <c r="G18">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H18">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I18">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>115</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19">
-        <v>-1</v>
-      </c>
-      <c r="E19">
-        <v>38</v>
-      </c>
-      <c r="F19">
-        <v>38</v>
-      </c>
-      <c r="G19">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H19">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I19">
-        <f t="shared" ca="1" si="2"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>116</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20">
-        <v>-1</v>
-      </c>
-      <c r="E20">
-        <v>38</v>
-      </c>
-      <c r="F20">
-        <v>38</v>
-      </c>
-      <c r="G20">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H20">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I20">
-        <f t="shared" ca="1" si="2"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21">
-        <v>-1</v>
-      </c>
-      <c r="E21">
-        <v>38</v>
-      </c>
-      <c r="F21">
-        <v>38</v>
-      </c>
-      <c r="G21">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H21">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I21">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>118</v>
-      </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22">
-        <v>-1</v>
-      </c>
-      <c r="E22">
-        <v>38</v>
-      </c>
-      <c r="F22">
-        <v>38</v>
-      </c>
-      <c r="G22">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H22">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I22">
-        <f t="shared" ca="1" si="2"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>119</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="D23">
-        <v>-1</v>
-      </c>
-      <c r="E23">
-        <v>39</v>
-      </c>
-      <c r="F23">
-        <v>39</v>
-      </c>
-      <c r="G23">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H23">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I23">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>120</v>
-      </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
-      <c r="D24">
-        <v>-1</v>
-      </c>
-      <c r="E24">
-        <v>39</v>
-      </c>
-      <c r="F24">
-        <v>39</v>
-      </c>
-      <c r="G24">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I24">
-        <f t="shared" ca="1" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>121</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-      <c r="D25">
-        <v>-1</v>
-      </c>
-      <c r="E25">
-        <v>39</v>
-      </c>
-      <c r="F25">
-        <v>39</v>
-      </c>
-      <c r="G25">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H25">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I25">
-        <f t="shared" ca="1" si="2"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>122</v>
-      </c>
-      <c r="C26">
-        <v>3</v>
-      </c>
-      <c r="D26">
-        <v>-1</v>
-      </c>
-      <c r="E26">
-        <v>39</v>
-      </c>
-      <c r="F26">
-        <v>39</v>
-      </c>
-      <c r="G26">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H26">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I26">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>123</v>
-      </c>
-      <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="D27">
-        <v>-1</v>
-      </c>
-      <c r="E27">
-        <v>39</v>
-      </c>
-      <c r="F27">
-        <v>39</v>
-      </c>
-      <c r="G27">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H27">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I27">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>151</v>
-      </c>
-      <c r="C28">
-        <v>3</v>
-      </c>
-      <c r="D28">
-        <v>-1</v>
-      </c>
-      <c r="E28">
-        <v>39</v>
-      </c>
-      <c r="F28">
-        <v>39</v>
-      </c>
-      <c r="G28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H28">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I28">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>152</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29">
-        <v>-1</v>
-      </c>
-      <c r="E29">
-        <v>7</v>
-      </c>
-      <c r="F29">
-        <v>7</v>
-      </c>
-      <c r="G29">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H29">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I29">
-        <f t="shared" ca="1" si="2"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>153</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="D30">
-        <v>-1</v>
-      </c>
-      <c r="E30">
-        <v>7</v>
-      </c>
-      <c r="F30">
-        <v>7</v>
-      </c>
-      <c r="G30">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H30">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I30">
-        <f t="shared" ca="1" si="2"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>154</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31">
-        <v>-1</v>
-      </c>
-      <c r="E31">
-        <v>7</v>
-      </c>
-      <c r="F31">
-        <v>7</v>
-      </c>
-      <c r="G31">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H31">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I31">
-        <f t="shared" ca="1" si="2"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>155</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <v>-1</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="G32">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H32">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I32">
-        <f t="shared" ca="1" si="2"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>156</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <v>-1</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H33">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I33">
-        <f t="shared" ca="1" si="2"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
-        <v>157</v>
-      </c>
-      <c r="C34">
-        <v>3</v>
-      </c>
-      <c r="D34">
-        <v>-1</v>
-      </c>
-      <c r="E34">
-        <v>19</v>
-      </c>
-      <c r="F34">
-        <v>3</v>
-      </c>
-      <c r="G34">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H34">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I34">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>158</v>
-      </c>
-      <c r="C35">
-        <v>2</v>
-      </c>
-      <c r="D35">
-        <v>-1</v>
-      </c>
-      <c r="E35">
-        <v>20</v>
-      </c>
-      <c r="F35">
-        <v>2</v>
-      </c>
-      <c r="G35">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H35">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I35">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
-        <v>159</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36">
-        <v>-1</v>
-      </c>
-      <c r="E36">
-        <v>3</v>
-      </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H36">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I36">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3745,7 +3721,7 @@
         <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3767,7 +3743,7 @@
         <v>65</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3778,7 +3754,7 @@
         <v>66</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3786,10 +3762,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3797,10 +3773,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3808,7 +3784,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>73</v>
@@ -3819,7 +3795,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>73</v>
@@ -3830,10 +3806,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3841,7 +3817,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>73</v>
@@ -3874,10 +3850,10 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3885,13 +3861,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1">
         <v>35</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3899,13 +3875,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" s="1">
         <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3913,13 +3889,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4" s="1">
         <v>38</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3927,13 +3903,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="1">
         <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3941,13 +3917,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="1">
         <v>-1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3955,13 +3931,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C7" s="1">
         <v>-1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3969,13 +3945,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8" s="1">
         <v>-1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -4022,7 +3998,7 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -4045,13 +4021,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented walking quests for player
</commit_message>
<xml_diff>
--- a/zzz_other/tables.xlsx
+++ b/zzz_other/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Filip\škola\!!!_MATRIP\DnD\zzz_other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C830230-E874-409B-9389-3589BC08C0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5206BE-1E9E-4AAF-9B3D-DFEAD1906C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6615" windowWidth="16440" windowHeight="28440" activeTab="2" xr2:uid="{75D15189-BFBB-4142-B930-759327EB73F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{75D15189-BFBB-4142-B930-759327EB73F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Předměty" sheetId="6" r:id="rId1"/>
@@ -251,9 +251,6 @@
     <t>U opilého poníka</t>
   </si>
   <si>
-    <t xml:space="preserve">Hrad </t>
-  </si>
-  <si>
     <t>Stanice hlídky</t>
   </si>
   <si>
@@ -780,6 +777,9 @@
   </si>
   <si>
     <t>Barman Brčko</t>
+  </si>
+  <si>
+    <t>Hrad</t>
   </si>
 </sst>
 </file>
@@ -1172,28 +1172,28 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" t="s">
         <v>140</v>
       </c>
-      <c r="E1" t="s">
-        <v>141</v>
-      </c>
       <c r="F1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1201,10 +1201,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2">
         <v>-2</v>
@@ -1216,16 +1216,16 @@
         <v>2000</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1233,10 +1233,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3">
         <v>-1</v>
@@ -1248,16 +1248,16 @@
         <v>500</v>
       </c>
       <c r="G3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1265,10 +1265,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4">
         <v>-3</v>
@@ -1280,16 +1280,16 @@
         <v>50</v>
       </c>
       <c r="G4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I4">
         <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1297,10 +1297,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1312,16 +1312,16 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1329,10 +1329,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1344,16 +1344,16 @@
         <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1361,10 +1361,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D7">
         <v>-1</v>
@@ -1376,16 +1376,16 @@
         <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1393,10 +1393,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D8">
         <v>-1</v>
@@ -1408,16 +1408,16 @@
         <v>69</v>
       </c>
       <c r="G8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1425,10 +1425,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9">
         <v>-1</v>
@@ -1440,16 +1440,16 @@
         <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1457,10 +1457,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D10">
         <v>-1</v>
@@ -1472,16 +1472,16 @@
         <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1489,10 +1489,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D11">
         <v>-1</v>
@@ -1504,16 +1504,16 @@
         <v>20</v>
       </c>
       <c r="G11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1521,10 +1521,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D12">
         <v>-1</v>
@@ -1536,16 +1536,16 @@
         <v>10</v>
       </c>
       <c r="G12" t="s">
+        <v>210</v>
+      </c>
+      <c r="H12" t="s">
         <v>211</v>
-      </c>
-      <c r="H12" t="s">
-        <v>212</v>
       </c>
       <c r="I12">
         <v>10</v>
       </c>
       <c r="J12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1553,10 +1553,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1568,16 +1568,16 @@
         <v>15</v>
       </c>
       <c r="G13" t="s">
+        <v>210</v>
+      </c>
+      <c r="H13" t="s">
         <v>211</v>
-      </c>
-      <c r="H13" t="s">
-        <v>212</v>
       </c>
       <c r="I13">
         <v>12</v>
       </c>
       <c r="J13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1585,10 +1585,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1600,16 +1600,16 @@
         <v>15</v>
       </c>
       <c r="G14" t="s">
+        <v>210</v>
+      </c>
+      <c r="H14" t="s">
         <v>211</v>
-      </c>
-      <c r="H14" t="s">
-        <v>212</v>
       </c>
       <c r="I14">
         <v>15</v>
       </c>
       <c r="J14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1617,10 +1617,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1632,16 +1632,16 @@
         <v>10</v>
       </c>
       <c r="G15" t="s">
+        <v>210</v>
+      </c>
+      <c r="H15" t="s">
         <v>211</v>
-      </c>
-      <c r="H15" t="s">
-        <v>212</v>
       </c>
       <c r="I15">
         <v>12</v>
       </c>
       <c r="J15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1649,10 +1649,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1664,16 +1664,16 @@
         <v>100</v>
       </c>
       <c r="G16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1681,10 +1681,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1696,16 +1696,16 @@
         <v>100</v>
       </c>
       <c r="G17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -1717,8 +1717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9C1193-21D4-4077-9037-2F33601C62B1}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1742,13 +1742,13 @@
         <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1765,13 +1765,13 @@
         <v>20</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -1788,11 +1788,11 @@
         <v>34</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1809,11 +1809,11 @@
         <v>52</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1827,16 +1827,16 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1853,11 +1853,11 @@
         <v>51</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1871,14 +1871,14 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1895,11 +1895,11 @@
         <v>55</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1916,11 +1916,11 @@
         <v>54</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1937,11 +1937,11 @@
         <v>48</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1958,11 +1958,11 @@
         <v>56</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1979,11 +1979,11 @@
         <v>50</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -2000,11 +2000,11 @@
         <v>58</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -2018,14 +2018,14 @@
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -2042,13 +2042,13 @@
         <v>38</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -2065,11 +2065,11 @@
         <v>37</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -2083,14 +2083,14 @@
         <v>12</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -2107,13 +2107,13 @@
         <v>36</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -2130,11 +2130,11 @@
         <v>47</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -2151,11 +2151,11 @@
         <v>61</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -2172,11 +2172,11 @@
         <v>53</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -2190,14 +2190,14 @@
         <v>15</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -2214,11 +2214,11 @@
         <v>45</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -2235,11 +2235,11 @@
         <v>60</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -2256,11 +2256,11 @@
         <v>41</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -2277,11 +2277,11 @@
         <v>44</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -2298,11 +2298,11 @@
         <v>39</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -2319,11 +2319,11 @@
         <v>35</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -2340,11 +2340,11 @@
         <v>40</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -2358,16 +2358,16 @@
         <v>23</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -2384,11 +2384,11 @@
         <v>46</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -2405,11 +2405,11 @@
         <v>59</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -2426,11 +2426,11 @@
         <v>29</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -2441,17 +2441,17 @@
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>69</v>
+        <v>245</v>
       </c>
       <c r="C34" s="1">
         <v>27</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2465,11 +2465,11 @@
         <v>49</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2483,11 +2483,11 @@
         <v>57</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2495,17 +2495,17 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C37" s="1">
         <v>12</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2513,19 +2513,19 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C38" s="1">
         <v>5</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2533,19 +2533,19 @@
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C39" s="1">
         <v>3</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2553,17 +2553,17 @@
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C40" s="1">
         <v>28</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2571,17 +2571,17 @@
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C41" s="1">
         <v>15</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2597,7 +2597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE42307A-777D-49E3-9DBB-1C926DF7AB9F}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
@@ -2620,7 +2620,7 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
         <v>67</v>
@@ -2629,13 +2629,13 @@
         <v>64</v>
       </c>
       <c r="F1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" t="s">
         <v>145</v>
       </c>
-      <c r="G1" t="s">
-        <v>146</v>
-      </c>
       <c r="H1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2656,15 +2656,15 @@
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G2">
         <f ca="1">RANDBETWEEN(1,5-F2)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H2">
         <f ca="1">RANDBETWEEN(10,70)</f>
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2672,7 +2672,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2685,15 +2685,15 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F37" ca="1" si="0">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G37" ca="1" si="1">RANDBETWEEN(1,5-F3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H36" ca="1" si="2">RANDBETWEEN(10,70)</f>
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2701,7 +2701,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -2714,7 +2714,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
@@ -2722,7 +2722,7 @@
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="2"/>
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2730,7 +2730,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -2743,7 +2743,7 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="1"/>
@@ -2751,7 +2751,7 @@
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="2"/>
-        <v>55</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2759,7 +2759,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2776,11 +2776,11 @@
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="2"/>
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2788,7 +2788,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -2809,7 +2809,7 @@
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="2"/>
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2817,7 +2817,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -2830,15 +2830,15 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="2"/>
-        <v>63</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2846,7 +2846,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -2863,11 +2863,11 @@
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="2"/>
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2875,7 +2875,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="1"/>
@@ -2896,7 +2896,7 @@
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2904,7 +2904,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -2917,15 +2917,15 @@
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2933,7 +2933,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -2946,15 +2946,15 @@
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="2"/>
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2962,7 +2962,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2979,11 +2979,11 @@
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="2"/>
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2991,7 +2991,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -3008,11 +3008,11 @@
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -3020,7 +3020,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="2"/>
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -3049,7 +3049,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -3070,7 +3070,7 @@
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="2"/>
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -3078,7 +3078,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -3091,7 +3091,7 @@
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
@@ -3099,7 +3099,7 @@
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -3107,7 +3107,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -3120,15 +3120,15 @@
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="2"/>
-        <v>58</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -3136,7 +3136,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -3153,11 +3153,11 @@
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -3165,7 +3165,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -3178,7 +3178,7 @@
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
@@ -3186,7 +3186,7 @@
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -3194,7 +3194,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -3207,7 +3207,7 @@
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
@@ -3215,7 +3215,7 @@
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="2"/>
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -3223,7 +3223,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -3236,7 +3236,7 @@
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
@@ -3244,7 +3244,7 @@
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="2"/>
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -3252,7 +3252,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -3273,7 +3273,7 @@
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="2"/>
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -3281,7 +3281,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -3302,7 +3302,7 @@
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -3310,7 +3310,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -3323,15 +3323,15 @@
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="2"/>
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -3339,7 +3339,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -3352,7 +3352,7 @@
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="1"/>
@@ -3360,7 +3360,7 @@
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -3368,7 +3368,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="1"/>
@@ -3389,7 +3389,7 @@
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="2"/>
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -3397,7 +3397,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -3410,15 +3410,15 @@
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="2"/>
-        <v>45</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3426,7 +3426,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -3439,7 +3439,7 @@
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="1"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="2"/>
-        <v>60</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -3455,7 +3455,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -3468,15 +3468,15 @@
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -3484,7 +3484,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -3497,15 +3497,15 @@
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3513,7 +3513,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3534,7 +3534,7 @@
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3542,7 +3542,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -3555,15 +3555,15 @@
       </c>
       <c r="F33">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3571,7 +3571,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C34">
         <v>3</v>
@@ -3584,7 +3584,7 @@
       </c>
       <c r="F34">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="1"/>
@@ -3592,7 +3592,7 @@
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="2"/>
-        <v>56</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3600,7 +3600,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -3613,15 +3613,15 @@
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3629,7 +3629,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -3642,15 +3642,15 @@
       </c>
       <c r="F36">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="2"/>
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3658,7 +3658,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C37">
         <v>5</v>
@@ -3671,15 +3671,15 @@
       </c>
       <c r="F37">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G37">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H37">
         <f ca="1">RANDBETWEEN(10,70)</f>
-        <v>16</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3710,7 +3710,7 @@
         <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3721,7 +3721,7 @@
         <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3729,10 +3729,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3743,7 +3743,7 @@
         <v>65</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3754,7 +3754,7 @@
         <v>66</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3762,10 +3762,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3773,10 +3773,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3784,10 +3784,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3795,10 +3795,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3806,10 +3806,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3817,10 +3817,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -3850,10 +3850,10 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3861,13 +3861,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="1">
         <v>35</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3875,13 +3875,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1">
         <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3889,13 +3889,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" s="1">
         <v>38</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3903,13 +3903,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="1">
         <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3917,13 +3917,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="1">
         <v>-1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3931,13 +3931,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" s="1">
         <v>-1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3945,13 +3945,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" s="1">
         <v>-1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -3998,7 +3998,7 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -4021,13 +4021,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>